<commit_message>
update format_input and input_files table
</commit_message>
<xml_diff>
--- a/resources/input_files.xlsx
+++ b/resources/input_files.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukefunk/packages/NatureProtocols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukefunk/packages/NatureProtocols/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9107370-030D-0146-BFF1-B6AE001372BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66654C1-DE54-364B-8F86-7EBF773EA850}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="-19000" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_ascp" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>original filename</t>
   </si>
@@ -68,21 +68,6 @@
     <t>B3</t>
   </si>
   <si>
-    <t>input_sbs/raw/10X_c4_B3_A594_Site-0.tif</t>
-  </si>
-  <si>
-    <t>input_sbs/raw/10X_c4_B3_CY3_Site-0.tif</t>
-  </si>
-  <si>
-    <t>input_sbs/raw/10X_c4_B3_CY5_Site-0.tif</t>
-  </si>
-  <si>
-    <t>input_sbs/raw/10X_c4_B3_CY7_Site-0.tif</t>
-  </si>
-  <si>
-    <t>input_sbs/raw/10X_c4_B3_DAPI_Site-0.tif</t>
-  </si>
-  <si>
     <t>DAPI</t>
   </si>
   <si>
@@ -96,6 +81,33 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c4_B3_A594_Site-0.tif</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c4_B3_CY3_Site-0.tif</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c4_B3_CY5_Site-0.tif</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c4_B3_CY7_Site-0.tif</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c4_B3_DAPI_Site-0.tif</t>
+  </si>
+  <si>
+    <t>c0-DAPI-GFP</t>
+  </si>
+  <si>
+    <t>input/raw/10X_c0-DAPI-GFP_B3_Site-0.tif</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>ALL</t>
   </si>
 </sst>
 </file>
@@ -374,19 +386,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="46.1640625" customWidth="1"/>
-    <col min="2" max="6" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="8" max="8" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -417,7 +431,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -435,16 +449,16 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5" t="str">
-        <f>"input/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"_Tile-"&amp;E2&amp;"."&amp;F2&amp;".tif"</f>
-        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_Tile-0.sbs.tif</v>
+        <f>IF(F2="sbs","input/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"_"&amp;D2&amp;"_Tile-"&amp;E2&amp;"."&amp;F2&amp;".tif","input/"&amp;B2&amp;"_"&amp;C2&amp;"/"&amp;B2&amp;"_"&amp;C2&amp;"_"&amp;D2&amp;"_Tile-"&amp;E2&amp;"."&amp;F2&amp;".tif")</f>
+        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_B3_Tile-0.sbs.tif</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -462,16 +476,16 @@
         <v>10</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5" t="str">
-        <f>"input/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"_Tile-"&amp;E3&amp;"."&amp;F3&amp;".tif"</f>
-        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_Tile-0.sbs.tif</v>
+        <f t="shared" ref="H3:H7" si="0">IF(F3="sbs","input/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"_"&amp;D3&amp;"_Tile-"&amp;E3&amp;"."&amp;F3&amp;".tif","input/"&amp;B3&amp;"_"&amp;C3&amp;"/"&amp;B3&amp;"_"&amp;C3&amp;"_"&amp;D3&amp;"_Tile-"&amp;E3&amp;"."&amp;F3&amp;".tif")</f>
+        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_B3_Tile-0.sbs.tif</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -489,16 +503,16 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H4" s="5" t="str">
-        <f>"input/"&amp;B4&amp;"_c"&amp;C4&amp;"-SBS-"&amp;C4&amp;"/"&amp;B4&amp;"_c"&amp;C4&amp;"-SBS-"&amp;C4&amp;"_Tile-"&amp;E4&amp;"."&amp;F4&amp;".tif"</f>
-        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_Tile-0.sbs.tif</v>
+        <f t="shared" si="0"/>
+        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_B3_Tile-0.sbs.tif</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -516,16 +530,16 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5" t="str">
-        <f>"input/"&amp;B5&amp;"_c"&amp;C5&amp;"-SBS-"&amp;C5&amp;"/"&amp;B5&amp;"_c"&amp;C5&amp;"-SBS-"&amp;C5&amp;"_Tile-"&amp;E5&amp;"."&amp;F5&amp;".tif"</f>
-        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_Tile-0.sbs.tif</v>
+        <f t="shared" si="0"/>
+        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_B3_Tile-0.sbs.tif</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -543,11 +557,38 @@
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f>"input/"&amp;B6&amp;"_c"&amp;C6&amp;"-SBS-"&amp;C6&amp;"/"&amp;B6&amp;"_c"&amp;C6&amp;"-SBS-"&amp;C6&amp;"_Tile-"&amp;E6&amp;"."&amp;F6&amp;".tif"</f>
-        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_Tile-0.sbs.tif</v>
+        <f t="shared" si="0"/>
+        <v>input/10X_c4-SBS-4/10X_c4-SBS-4_B3_Tile-0.sbs.tif</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>input/10X_c0-DAPI-GFP/10X_c0-DAPI-GFP_B3_Tile-0.phenotype.tif</v>
       </c>
     </row>
   </sheetData>

</xml_diff>